<commit_message>
published state of ETDataset on 11th of June  2018
</commit_message>
<xml_diff>
--- a/nodes_source_analyses/energy/energy_hydrogen_solar_pv_solar_radiation.central_producer.xlsx
+++ b/nodes_source_analyses/energy/energy_hydrogen_solar_pv_solar_radiation.central_producer.xlsx
@@ -5,12 +5,12 @@
   <workbookPr showInkAnnotation="0" codeName="ThisWorkbook" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marliekeverweij/Projects/etdataset/nodes_source_analyses/energy/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michieldenhaan/Projects/etdataset/nodes_source_analyses/energy/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7EA1B8-63E5-1949-B691-7B3C7A9C680E}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B3D900E-C2D8-7C4C-9794-1E7E946508CF}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="26820" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13400" yWindow="460" windowWidth="25600" windowHeight="26820" tabRatio="762" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover sheet" sheetId="14" r:id="rId1"/>
@@ -37,7 +37,7 @@
     <definedName name="Wp_to_kWp">#REF!</definedName>
     <definedName name="WP_to_MWp">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="181">
   <si>
     <t>Source</t>
   </si>
@@ -760,6 +760,12 @@
   </si>
   <si>
     <t>Fraunhofer 2015 p.40</t>
+  </si>
+  <si>
+    <t>moved cost of installing to initial investment costs</t>
+  </si>
+  <si>
+    <t>Installation costs set to 0, they are added to initial investment</t>
   </si>
 </sst>
 </file>
@@ -1695,7 +1701,7 @@
     <xf numFmtId="43" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="39" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="217">
+  <cellXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2067,6 +2073,8 @@
     <xf numFmtId="0" fontId="37" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="310">
     <cellStyle name="Comma" xfId="308" builtinId="3"/>
@@ -3447,7 +3455,7 @@
   <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A18:XFD22"/>
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -3766,7 +3774,7 @@
       </c>
       <c r="E20" s="36">
         <f>'Research data'!H15</f>
-        <v>16420000</v>
+        <v>17420000</v>
       </c>
       <c r="F20" s="30"/>
       <c r="G20" s="30" t="s">
@@ -3809,15 +3817,15 @@
       </c>
       <c r="E22" s="78">
         <f>'Research data'!H20</f>
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="F22" s="30"/>
       <c r="G22" s="30" t="s">
         <v>26</v>
       </c>
       <c r="H22" s="30"/>
-      <c r="I22" s="158" t="s">
-        <v>107</v>
+      <c r="I22" s="218" t="s">
+        <v>180</v>
       </c>
       <c r="J22" s="129"/>
     </row>
@@ -4310,7 +4318,7 @@
   <dimension ref="B1:O27"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16"/>
@@ -4628,14 +4636,14 @@
       </c>
       <c r="G15" s="122"/>
       <c r="H15" s="165">
-        <f>H16*H7*1000</f>
-        <v>16420000</v>
+        <f>K15</f>
+        <v>17420000</v>
       </c>
       <c r="I15" s="166"/>
       <c r="J15" s="50"/>
       <c r="K15" s="167">
-        <f>K16*H7*1000</f>
-        <v>16420000</v>
+        <f>K16*H7*1000+K20</f>
+        <v>17420000</v>
       </c>
       <c r="L15" s="61"/>
       <c r="M15" s="32"/>
@@ -4749,8 +4757,7 @@
       </c>
       <c r="G20" s="121"/>
       <c r="H20" s="55">
-        <f>K20</f>
-        <v>1000000</v>
+        <v>0</v>
       </c>
       <c r="I20" s="50"/>
       <c r="J20" s="50"/>
@@ -4761,7 +4768,9 @@
       <c r="L20" s="50"/>
       <c r="M20" s="32"/>
       <c r="N20" s="32"/>
-      <c r="O20" s="139"/>
+      <c r="O20" s="217" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="21" spans="2:15" ht="17" thickBot="1">
       <c r="B21" s="34"/>

</xml_diff>